<commit_message>
Add SPB Bolid and new GUI
</commit_message>
<xml_diff>
--- a/БД.xlsx
+++ b/БД.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\-\I.Sushkov\PycharmProjects\skud-report-structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C42C0EB-60F2-48FB-BB79-0B04FEA66C78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870334B7-3D3F-4E01-9387-9B0406D0AB1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="157">
   <si>
     <t>Отдел</t>
   </si>
@@ -377,9 +377,6 @@
     <t>Управление делами</t>
   </si>
   <si>
-    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\АКТИВ\Автотранспортный отдел\</t>
-  </si>
-  <si>
     <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\АКТИВ\Административно-режимный отдел\</t>
   </si>
   <si>
@@ -471,6 +468,42 @@
   </si>
   <si>
     <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\СК\Отдел по работе с клиентами\</t>
+  </si>
+  <si>
+    <t>Производственно-технический отдел</t>
+  </si>
+  <si>
+    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\АКТИВ\Производственно-технический отдел\</t>
+  </si>
+  <si>
+    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\АКТИВ\Управление по взаимодействию с государственными органами власти\</t>
+  </si>
+  <si>
+    <t>Управление по взаимодействию с государственными органами власти</t>
+  </si>
+  <si>
+    <t>Сметно-аналитический отдел</t>
+  </si>
+  <si>
+    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\АКТИВ\Сметно-аналитический отдел\</t>
+  </si>
+  <si>
+    <t>Питер (БВРЗ)</t>
+  </si>
+  <si>
+    <t>Участок автотранспорта</t>
+  </si>
+  <si>
+    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\БВРЗ\Руководство\</t>
+  </si>
+  <si>
+    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\БВРЗ\Участок автотранспорта\</t>
+  </si>
+  <si>
+    <t>Питер (УК)</t>
+  </si>
+  <si>
+    <t>N:\АКТИВ\УКБ\Отчеты СКУД\СПБ\УК\Автотранспортный отдел\</t>
   </si>
 </sst>
 </file>
@@ -523,7 +556,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -576,29 +609,18 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -607,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -635,29 +657,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,69 +984,85 @@
     <col min="16" max="16" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="24" customWidth="1"/>
     <col min="18" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="24" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" customWidth="1"/>
+    <col min="21" max="21" width="32.85546875" customWidth="1"/>
+    <col min="22" max="22" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-    </row>
-    <row r="2" spans="1:18" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+    </row>
+    <row r="2" spans="1:22" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="11" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="R2" s="12"/>
-    </row>
-    <row r="3" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="L2" s="14"/>
+      <c r="M2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="14"/>
+      <c r="O2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="R2" s="14"/>
+      <c r="S2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="T2" s="14"/>
+      <c r="U2" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="V2" s="14"/>
+    </row>
+    <row r="3" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1082,8 +1117,20 @@
       <c r="R3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+      <c r="S3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1162,7 @@
         <v>39</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>114</v>
@@ -1124,22 +1171,34 @@
         <v>12</v>
       </c>
       <c r="N4" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="O4" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="P4" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R4" s="17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="R4" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>63</v>
       </c>
@@ -1170,26 +1229,32 @@
       <c r="J5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>16</v>
+      <c r="K5" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>115</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="R5" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -1217,19 +1282,19 @@
         <v>41</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>116</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>65</v>
       </c>
@@ -1252,20 +1317,20 @@
       <c r="H7" s="7"/>
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="3" t="s">
-        <v>123</v>
+      <c r="K7" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>117</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="56.25" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1289,19 +1354,19 @@
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>118</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="75" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>66</v>
       </c>
@@ -1325,19 +1390,19 @@
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
       <c r="K9" s="5" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>119</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="93.75" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>67</v>
       </c>
@@ -1360,20 +1425,20 @@
       <c r="H10" s="7"/>
       <c r="I10" s="6"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="5" t="s">
-        <v>124</v>
+      <c r="K10" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>120</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="75" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>68</v>
       </c>
@@ -1396,14 +1461,14 @@
       <c r="H11" s="7"/>
       <c r="I11" s="6"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="3" t="s">
-        <v>113</v>
+      <c r="K11" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="75" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>69</v>
       </c>
@@ -1427,13 +1492,13 @@
       <c r="I12" s="6"/>
       <c r="J12" s="7"/>
       <c r="K12" s="5" t="s">
-        <v>38</v>
+        <v>145</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="93.75" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>70</v>
       </c>
@@ -1456,9 +1521,14 @@
       <c r="H13" s="7"/>
       <c r="I13" s="6"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:18" ht="75" x14ac:dyDescent="0.3">
+      <c r="K13" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>71</v>
       </c>
@@ -1481,9 +1551,14 @@
       <c r="H14" s="7"/>
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:18" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="K14" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
@@ -1503,7 +1578,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:18" ht="75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="75" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
@@ -1732,17 +1807,19 @@
       <c r="B36" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="E1:R1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="K2:L2"/>
+  <mergeCells count="12">
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="U2:V2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DB change ADD PIIR b PYL
</commit_message>
<xml_diff>
--- a/БД.xlsx
+++ b/БД.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\-\I.Sushkov\PycharmProjects\skud-report-structure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i.slavianskiy\Documents\skud-report-structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD5C2A5-4BED-4D4F-81B0-1121C1C13B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32910" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="345" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$K$1:$K$42</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="279">
   <si>
     <t>Отдел</t>
   </si>
@@ -200,9 +203,6 @@
     <t>Отдел по работе с клиентами</t>
   </si>
   <si>
-    <t>Питер (CR)</t>
-  </si>
-  <si>
     <t>Производственно-технический отдел</t>
   </si>
   <si>
@@ -242,9 +242,6 @@
     <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Управление по развитию активов\</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Управление по инвестиционной деятельности\Сметно-аналитический отдел\</t>
-  </si>
-  <si>
     <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Управление по развитию активов\Отдел главного механика\</t>
   </si>
   <si>
@@ -359,9 +356,6 @@
     <t>Отдел экономической безопасности</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридическое управление\</t>
-  </si>
-  <si>
     <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Администрация\</t>
   </si>
   <si>
@@ -431,9 +425,6 @@
     <t>Отдел по контролю за техническим состоянием парка грузовых вагонов</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\УК\Бухгалтерия\</t>
-  </si>
-  <si>
     <t xml:space="preserve">Управление по взаимодействию с государственными органами власти </t>
   </si>
   <si>
@@ -479,9 +470,6 @@
     <t>Отдел дноуглубительных работ</t>
   </si>
   <si>
-    <t>Отдел охраны окружающей среды</t>
-  </si>
-  <si>
     <t>Управление информационных технологий</t>
   </si>
   <si>
@@ -527,9 +515,6 @@
     <t>N:\УК\УКБ\Отчеты СКУД\УК\Управление корпоративной безопасности\Автотранспортный отдел\</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\УК\Управление внутреннего аудита\</t>
-  </si>
-  <si>
     <t>N:\УК\УКБ\Отчеты СКУД\УК\Управление кадров\</t>
   </si>
   <si>
@@ -584,15 +569,9 @@
     <t>Геодезический отдел</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Геодезический отдел\</t>
-  </si>
-  <si>
     <t>Отдел по организации строительного контроля заказчика</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Отдел по организации строительного контроля заказчика\</t>
-  </si>
-  <si>
     <t>Отдел сопровождения строительства</t>
   </si>
   <si>
@@ -602,27 +581,12 @@
     <t>Производственный отдел</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Производственный отдел\</t>
-  </si>
-  <si>
     <t>Сметно-договорной отдел</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Сметно-договорной отдел\</t>
-  </si>
-  <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Управление по развитию активов\Отдел главного механика\</t>
-  </si>
-  <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Управление по развитию активов\Отдел главного энергетика\</t>
-  </si>
-  <si>
     <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Управление по развитию активов\Отдел организации дноуглубительных работ\</t>
   </si>
   <si>
-    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Управление по развитию активов\Отдел охраны окружающей среды\</t>
-  </si>
-  <si>
     <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Управление по развитию активов\Производственно-технический отдел\</t>
   </si>
   <si>
@@ -633,12 +597,288 @@
   </si>
   <si>
     <t>N:\УК\УКБ\Отчеты СКУД\СПБ\БВРЗ\Лаборатория неразрушающего контроля\</t>
+  </si>
+  <si>
+    <t>Департамент по бухгалтерскому, налоговому учету и аудиту</t>
+  </si>
+  <si>
+    <t>Управление по расчету заработной платы</t>
+  </si>
+  <si>
+    <t>Управление по учету и отчетности управляющей компании</t>
+  </si>
+  <si>
+    <t>Управление по учету ключевых активов</t>
+  </si>
+  <si>
+    <t>Управление по учету непрофильных компаний</t>
+  </si>
+  <si>
+    <t>Управление по учету перевозок</t>
+  </si>
+  <si>
+    <t>Управление по учету портовых инвестиций</t>
+  </si>
+  <si>
+    <t>Управление по учету ремонтов подвижного состава</t>
+  </si>
+  <si>
+    <t>Управление по учету строительства</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление внутреннего аудита\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по расчету заработной платы\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету и отчетности управляющей компании\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету ключевых активов\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету непрофильных компаний\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету перевозок\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету портовых инвестиций\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету ремонтов подвижного состава\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету строительства\</t>
+  </si>
+  <si>
+    <t>Управление по учету стивидорной деятельности</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету непрофильных компаний\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\УК\Департамент по бухгалтерскому, налоговому учету и аудиту\Управление по учету стивидорной деятельности\</t>
+  </si>
+  <si>
+    <t>Дирекция по орагнизации строительства</t>
+  </si>
+  <si>
+    <t>Управление главного инженера</t>
+  </si>
+  <si>
+    <t>Управление материально-технического обеспечения</t>
+  </si>
+  <si>
+    <t>Управление строительства</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\Геодезический отдел\</t>
+  </si>
+  <si>
+    <t>Отдел гидротехнических сооружений</t>
+  </si>
+  <si>
+    <t>Отдел оперативного планирования</t>
+  </si>
+  <si>
+    <t>Отдел гидротехнических сооружений и дноуглубительных работ</t>
+  </si>
+  <si>
+    <t>Отдел охраны окуржающей среды</t>
+  </si>
+  <si>
+    <t>Дирекция по экономике и финансам</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по экономике и финансам\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по управлению терминалом\Служба главного инженера\Отдел главного энергетика\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по управлению терминалом\Служба главного инженера\Отдел главного механика\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по управлению терминалом\Служба главного инженера\Отдел гидротехнических сооружений и дноуглубительных работ\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по экономике и финансам\</t>
+  </si>
+  <si>
+    <t>Дирекция по управлению терминалом</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по управлению терминалом\</t>
+  </si>
+  <si>
+    <t>Служба технического развития и контроля</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление главного инженера\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление материально-технического обеспечения\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\Отдел гидротехнических сооружений\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по управлению терминалом\Служба технического развития и контроля\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по организации строительства\Управление материально-технического обеспечения\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по организации строительства\Управление главного инженера\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по организации строительства\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по управлению терминалом\Служба технического развития и контроля\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\Отдел оперативного планирования\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по управлению терминалом\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\Сметно-договорной отдел\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\Производственный отдел\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по организации строительства\Управление строительства\Отдел по организации строительного контроля заказчика\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\АКТИВ\Дирекция по управлению терминалом\Служба технического развития и контроля\Отдел охраны окружающей среды\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент маркетинга\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\Управление правового сопровождения инвестиций\</t>
+  </si>
+  <si>
+    <t>Управление правового сопровождения инвестиций</t>
+  </si>
+  <si>
+    <t>Управление корпоративного развития</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\Управление корпоративного развития\</t>
+  </si>
+  <si>
+    <t>Управление правового сопровождения перевозок</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\Управление правового сопровождения перевозок\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\Судебно-правовое управление\</t>
+  </si>
+  <si>
+    <t>Судебно-правовое управление</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\</t>
+  </si>
+  <si>
+    <t>Юридический департамент</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Управление строительным проектом\</t>
+  </si>
+  <si>
+    <t>Управление строительным проектом</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\Судебно-правовое управление\Юридический отдел\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\УК\Управление кадров\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Юридический департамент\Судебно-правовое управление\Судебно-претензионный отдел\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\АКТИВ\Дирекция по организации строительства\Управление строительства\Сметно-аналитический отдел\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\ПУЛ\Администрация\</t>
+  </si>
+  <si>
+    <t>ПИИР</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\ПИИР\Руководство\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\ПИИР\Служба авторского надзора\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\ПИИР\Технический отдел\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\ПИИР\Бюро главных инженеров проектов\</t>
+  </si>
+  <si>
+    <t>Бюро главных инженеров проектов</t>
+  </si>
+  <si>
+    <t>Служба авторского надзора</t>
+  </si>
+  <si>
+    <t>Технический отдел</t>
+  </si>
+  <si>
+    <t>Питер (ПИИР)</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\ПИИР\Бюро главных инженеров проектов\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\ПИИР\Руководство\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\ПИИР\Служба авторского надзора\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\СПБ\ПИИР\Технический отдел\</t>
+  </si>
+  <si>
+    <t>Питер (ПУЛ)</t>
+  </si>
+  <si>
+    <t>Питер (СК)</t>
+  </si>
+  <si>
+    <t>Отдел по организации мероприятий и корпоративной социальной ответственности</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Управление по корпоративным коммуникациям\Отдел по организации мероприятий и корпоративной социальной ответственности\</t>
+  </si>
+  <si>
+    <t>N:\УК\УКБ\Отчеты СКУД\УК\Департамент стратегического развития и управления рисками\</t>
+  </si>
+  <si>
+    <t>Департамент стратегического развития и управления рисками</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -671,7 +911,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,8 +924,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -765,11 +1011,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -802,6 +1070,42 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1097,11 +1401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,93 +1434,117 @@
     <col min="24" max="24" width="28.28515625" customWidth="1"/>
     <col min="25" max="25" width="24.42578125" customWidth="1"/>
     <col min="26" max="26" width="24.7109375" customWidth="1"/>
+    <col min="27" max="27" width="21.5703125" customWidth="1"/>
+    <col min="28" max="28" width="20" customWidth="1"/>
+    <col min="29" max="29" width="15.28515625" customWidth="1"/>
+    <col min="30" max="30" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" customWidth="1"/>
+    <col min="32" max="32" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:32" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-    </row>
-    <row r="2" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+    </row>
+    <row r="2" spans="1:32" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="13" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="13" t="s">
+      <c r="J2" s="26"/>
+      <c r="K2" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="13" t="s">
+      <c r="N2" s="26"/>
+      <c r="O2" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="13" t="s">
+      <c r="P2" s="26"/>
+      <c r="Q2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="V2" s="14"/>
-      <c r="W2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="Z2" s="14"/>
-    </row>
-    <row r="3" spans="1:26" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="R2" s="26"/>
+      <c r="S2" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="T2" s="26"/>
+      <c r="U2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="V2" s="26"/>
+      <c r="W2" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="AF2" s="26"/>
+    </row>
+    <row r="3" spans="1:32" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1295,105 +1623,141 @@
       <c r="Z3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+      <c r="AA3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>46</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="X4" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="Z4" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="93.75" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1401,69 +1765,81 @@
         <v>6</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>132</v>
+        <v>196</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>47</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>54</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V5" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="W5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="X5" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="Z5" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="90" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD5" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF5" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
@@ -1471,435 +1847,495 @@
         <v>7</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>183</v>
+        <v>210</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>48</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="Z6" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="105" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="AD6" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="AF6" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="4"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="1" t="s">
-        <v>42</v>
+      <c r="K7" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>97</v>
+        <v>198</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>185</v>
+        <v>211</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>49</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="W7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="Z7" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="90" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="AD7" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>165</v>
+      <c r="K8" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>187</v>
+        <v>212</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>50</v>
       </c>
       <c r="R8" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="W8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="Z8" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="93.75" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>258</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="3" t="s">
-        <v>99</v>
+        <v>190</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>98</v>
+        <v>200</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="112.5" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="K10" s="3" t="s">
-        <v>101</v>
+        <v>191</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>191</v>
+        <v>201</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="93.75" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="3" t="s">
-        <v>12</v>
+        <v>192</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>176</v>
+        <v>215</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="W11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="93.75" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="1" t="s">
-        <v>8</v>
+      <c r="K12" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>43</v>
+        <v>203</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="112.5" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="X12" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
       <c r="K13" s="3" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>103</v>
+        <v>204</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>58</v>
+        <v>180</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="93.75" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="X13" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>234</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N14" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="K14" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="W14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>94</v>
+        <v>78</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="75" x14ac:dyDescent="0.3">
+      <c r="K15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="150" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1907,25 +2343,31 @@
       <c r="H16" s="5"/>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N16" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="K16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="105" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>225</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1934,21 +2376,25 @@
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
       <c r="K17" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>194</v>
+        <v>96</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>231</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1956,41 +2402,45 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+        <v>98</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="C19" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>233</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="93.75" x14ac:dyDescent="0.3">
+      <c r="K19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="105" x14ac:dyDescent="0.3">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1999,11 +2449,17 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>170</v>
+      <c r="K20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="N20" s="9" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="93.75" x14ac:dyDescent="0.3">
@@ -2015,14 +2471,20 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="131.25" x14ac:dyDescent="0.3">
+      <c r="K21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="93.75" x14ac:dyDescent="0.3">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -2032,13 +2494,19 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="10" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="56.25" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="93.75" x14ac:dyDescent="0.3">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -2047,14 +2515,20 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="K23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="N23" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="93.75" x14ac:dyDescent="0.3">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -2064,13 +2538,19 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="3" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="N24" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="112.5" x14ac:dyDescent="0.3">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -2079,19 +2559,194 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="K25" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="112.5" x14ac:dyDescent="0.3">
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
+      <c r="K26" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="K27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="N27" s="19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="K28" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="K29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="M29" s="23"/>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" spans="1:14" ht="131.25" x14ac:dyDescent="0.25">
+      <c r="K30" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="N30" s="24"/>
+    </row>
+    <row r="31" spans="1:14" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="K31" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L31" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="M31" s="23"/>
+      <c r="N31" s="24"/>
+    </row>
+    <row r="32" spans="1:14" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="K32" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="L32" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="N32" s="24"/>
+    </row>
+    <row r="33" spans="11:14" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="K33" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="L33" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="M33" s="23"/>
+      <c r="N33" s="24"/>
+    </row>
+    <row r="34" spans="11:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="K34" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="L34" s="21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="11:14" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="K35" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="L35" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="11:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="K36" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="L36" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="11:14" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="K37" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="21" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="38" spans="11:14" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="K38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39" spans="11:14" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="K39" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="L39" s="21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="40" spans="11:14" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="K40" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="L40" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="11:14" ht="150" x14ac:dyDescent="0.25">
+      <c r="K41" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="L41" s="21" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="42" spans="11:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="K42" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="L42" s="21" t="s">
+        <v>277</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="A1:Z1"/>
     <mergeCell ref="U2:V2"/>
     <mergeCell ref="W2:X2"/>
     <mergeCell ref="A2:B2"/>
@@ -2104,6 +2759,8 @@
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>